<commit_message>
reverted to a previous iteration that only handles one placeholder
</commit_message>
<xml_diff>
--- a/OutputFiles/game_outlines.xlsx
+++ b/OutputFiles/game_outlines.xlsx
@@ -443,828 +443,846 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>﻿H1: Lady Fortune Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Lady Fortune Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Lady Fortune Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Lady Fortune Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Lady Fortune Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Lady Fortune Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Lady Fortune Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Lady Fortune Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Lady Fortune Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>﻿H1: Black Wolf 2 Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Black Wolf 2 Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Black Wolf 2 Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Black Wolf 2 Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Black Wolf 2 Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Black Wolf 2 Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Black Wolf 2 Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Black Wolf 2 Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Black Wolf 2 Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>﻿H1: Fish Reef Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Fish Reef Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Fish Reef Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Fish Reef Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Fish Reef Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Fish Reef Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Fish Reef Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Fish Reef Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Fish Reef Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>﻿H1: Magic Ball Multichance Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Magic Ball Multichance Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Magic Ball Multichance Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Magic Ball Multichance Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Magic Ball Multichance Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Magic Ball Multichance Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Magic Ball Multichance Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Magic Ball Multichance Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Magic Ball Multichance Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>﻿H1: Wukong Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Wukong Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Wukong Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Wukong Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Wukong Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Wukong Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Wukong Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Wukong Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Wukong Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>﻿H1: Wolf Night Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Wolf Night Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Wolf Night Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Wolf Night Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Wolf Night Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Wolf Night Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Wolf Night Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Wolf Night Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Wolf Night Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>﻿H1: Tiger Gems Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Tiger Gems Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Tiger Gems Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Tiger Gems Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Tiger Gems Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Tiger Gems Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Tiger Gems Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Tiger Gems Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Tiger Gems Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>﻿H1: Moon Sisters Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Moon Sisters Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Moon Sisters Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Moon Sisters Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Moon Sisters Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Moon Sisters Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Moon Sisters Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Moon Sisters Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Moon Sisters Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>﻿H1: Mummy Power Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Mummy Power Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Mummy Power Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Mummy Power Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Mummy Power Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Mummy Power Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Mummy Power Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Mummy Power Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Mummy Power Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>﻿H1: Little Farm Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Little Farm Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Little Farm Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Little Farm Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Little Farm Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Little Farm Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Little Farm Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Little Farm Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Little Farm Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>﻿H1: Grab the Gold! Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Grab the Gold! Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Grab the Gold! Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Grab the Gold! Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Grab the Gold! Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Grab the Gold! Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Grab the Gold! Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Grab the Gold! Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Grab the Gold! Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>﻿H1: Rio Gems Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Rio Gems Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Rio Gems Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Rio Gems Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Rio Gems Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Rio Gems Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Rio Gems Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Rio Gems Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Rio Gems Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>﻿H1: Thunder of Olympus Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Thunder of Olympus Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Thunder of Olympus Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Thunder of Olympus Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Thunder of Olympus Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Thunder of Olympus Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Thunder of Olympus Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Thunder of Olympus Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Thunder of Olympus Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>﻿H1: Tiger's Gold Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Tiger's Gold Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Tiger's Gold Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Tiger's Gold Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Tiger's Gold Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Tiger's Gold Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Tiger's Gold Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Tiger's Gold Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Tiger's Gold Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>﻿H1: Wolf Saga Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Wolf Saga Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Wolf Saga Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Wolf Saga Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Wolf Saga Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Wolf Saga Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Wolf Saga Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Wolf Saga Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Wolf Saga Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>﻿H1: Gold Nuggets Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Gold Nuggets Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Gold Nuggets Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Gold Nuggets Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Gold Nuggets Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Gold Nuggets Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Gold Nuggets Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Gold Nuggets Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Gold Nuggets Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>﻿H1: Tiger Stone Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Tiger Stone Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Tiger Stone Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Tiger Stone Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Tiger Stone Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Tiger Stone Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Tiger Stone Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Tiger Stone Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Tiger Stone Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>﻿H1: Maya Sun Slots
-Introduction: Set the Stage
-* Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
-* Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
+          <t xml:space="preserve">H1: Maya Sun Slots
+Introduction: Set the Stage
+Start with an engaging hook to immediately capture the reader's attention. This could be a question, a surprising fact about the slot game industry, or an anecdote related to slot games' themes or history.
+Briefly introduce the slot game, mentioning its developer and its place within the broader context of online gaming.
 H2: Slots Game Maya Sun Theme &amp; Design
 Deep Dive into Theme and Design
-* Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
-* Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
-* Mention the audio effects and how they complement the game's visuals.
+Discuss the game's theme and how it compares to other slot games with similar themes. Highlight what sets this game apart in terms of its thematic execution and appeal.
+Describe the design elements (e.g., colors, symbols, animations) in vivid detail, giving the reader a vivid picture of the gaming experience.
+Mention the audio effects and how they complement the game's visuals.
 H2: Maya Sun Slots Features
 Features Exploration with Examples
-* Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
-* Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
+Elaborate on the game's features, providing scenarios or examples of when these features enhance gameplay. Discuss the impact of these features on the player's experience.
+Highlight strategic gameplay elements introduced by features like wilds, scatters, or unique mechanics.
 H2: Maya Sun Slot Game Payouts
 Analytical Payouts Section
-* Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
-* Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
-* Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
+Discuss the game's payout structure and compare it with industry standards. Offer insights into how the game's volatility affects the payout experience.
+Addition: Include a detailed table of symbols, descriptions, and their payout values, offering readers a comprehensive view of potential winnings.
+Addition: Include a visual diagram of the game's paylines. Use a table with reels as columns, marking 'X' for payline positions and '-' for non-payline positions, along with a description for each payline to visually demonstrate how wins are determined.
 H2: Maya Sun Slots RTP &amp; Volatility
 RTP &amp; Volatility: Provide Context
-* Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
+Explain the Return to Player (RTP) percentage and the game's volatility. Compare these aspects to other popular slot games to give readers a benchmark for what to expect.
 H2: How to Play Maya Sun Slots
 Playing Guide with Insider Tips
-* Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
-* Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
+Offer a simple, step-by-step guide to playing the slot, complemented by insider tips or strategies for enhancing the gaming experience.
+Addition: Discuss payline strategies, leveraging the visual payline diagram to inform these tactics.
 H2: How to Win at Maya Sun Slots
 Winning Strategies: Add Depth
-* Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
-* Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
-* Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
+Provide a detailed, in-depth strategy guide that provides clear steps to the reader. This should be aimed at improving the odds of winning significant payouts. This guide should include specific tactics related to bet levels, paylines, and feature utilization, supported by statistical insights where possible.
+Move beyond general advice to cover game-specific strategies that can make a tangible difference in winning outcomes.
+Give a direct answer as to the ideal strategy to maximize wins. General advice is not helpful or engaging. The user wants an edge let’s give it to them
 H2: Maya Sun Slots Free Spins
 Discuss Free Spins 
-* explore how the free spins impacts the gameplay and player expectations.
-H2: Pros &amp; Cons
-Pros &amp; Cons: Offer a Balanced View
-* Provide a nuanced discussion of the game's advantages and disadvantages
-* Create a table with a column for pros and a column for cons and include at least 5 pros and cons
-H2: Overall Review
-Overall Review
-* Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing</t>
+explore how the free spins impacts the gameplay and player expectations.
+H2: Pros &amp; Cons
+Pros &amp; Cons: Offer a Balanced View
+Provide a nuanced discussion of the game's advantages and disadvantages
+Create a table with a column for pros and a column for cons and include at least 5 pros and cons
+H2: Overall Review
+Overall Review
+Give an in depth overall review of the slot game. Write it as a person and include examples of emulated first hand experience that share a personal experience with the players and help them see if this game is worth playing 
+</t>
         </is>
       </c>
     </row>

</xml_diff>